<commit_message>
requirements.txt addition - G15
</commit_message>
<xml_diff>
--- a/resources/excel/25072024-Disney's_Animal_Kingdom.xlsx
+++ b/resources/excel/25072024-Disney's_Animal_Kingdom.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F109"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3461,10 +3461,8 @@
           <t>Avatar Flight of Passage</t>
         </is>
       </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>105</t>
-        </is>
+      <c r="F101" t="n">
+        <v>105</v>
       </c>
     </row>
     <row r="102">
@@ -3493,10 +3491,8 @@
           <t>DINOSAUR</t>
         </is>
       </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
+      <c r="F102" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="103">
@@ -3525,10 +3521,8 @@
           <t>Expedition Everest</t>
         </is>
       </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
+      <c r="F103" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="104">
@@ -3557,10 +3551,8 @@
           <t>It's Tough to be a Bug!</t>
         </is>
       </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="F104" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="105">
@@ -3589,10 +3581,8 @@
           <t>Kali River Rapids</t>
         </is>
       </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
+      <c r="F105" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="106">
@@ -3621,10 +3611,8 @@
           <t>Kilimanjaro Safaris</t>
         </is>
       </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="F106" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="107">
@@ -3653,10 +3641,8 @@
           <t>Meet Favorite Disney Pals at Adventurers Outpost</t>
         </is>
       </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+      <c r="F107" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="108">
@@ -3685,10 +3671,8 @@
           <t>Na'vi River Journey</t>
         </is>
       </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="F108" t="n">
+        <v>80</v>
       </c>
     </row>
     <row r="109">
@@ -3717,7 +3701,563 @@
           <t>TriceraTop Spin</t>
         </is>
       </c>
-      <c r="F109" t="inlineStr">
+      <c r="F109" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>13:15:12</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Pandora - The World of Avatar</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Avatar Flight of Passage</t>
+        </is>
+      </c>
+      <c r="F110" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>13:15:12</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Dinoland USA</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>DINOSAUR</t>
+        </is>
+      </c>
+      <c r="F111" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>13:15:12</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Asia</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Expedition Everest</t>
+        </is>
+      </c>
+      <c r="F112" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>13:15:12</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Discovery Island</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>It's Tough to be a Bug!</t>
+        </is>
+      </c>
+      <c r="F113" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>13:15:12</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Asia</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Kali River Rapids</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>13:15:12</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Africa</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Kilimanjaro Safaris</t>
+        </is>
+      </c>
+      <c r="F115" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>13:15:12</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Discovery Island</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Meet Favorite Disney Pals at Adventurers Outpost</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>13:15:12</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Pandora - The World of Avatar</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Na'vi River Journey</t>
+        </is>
+      </c>
+      <c r="F117" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>13:15:12</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Dinoland USA</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>TriceraTop Spin</t>
+        </is>
+      </c>
+      <c r="F118" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>13:20:26</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Pandora - The World of Avatar</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Avatar Flight of Passage</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>105</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>13:20:26</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Dinoland USA</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>DINOSAUR</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>13:20:26</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Asia</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Expedition Everest</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>13:20:26</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Discovery Island</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>It's Tough to be a Bug!</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>13:20:26</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Asia</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Kali River Rapids</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>13:20:26</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Africa</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Kilimanjaro Safaris</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>13:20:26</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Discovery Island</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Meet Favorite Disney Pals at Adventurers Outpost</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>13:20:26</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Pandora - The World of Avatar</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Na'vi River Journey</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>13:20:26</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Disney's Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Dinoland USA</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>TriceraTop Spin</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
         <is>
           <t>5</t>
         </is>

</xml_diff>